<commit_message>
updates to int stats
</commit_message>
<xml_diff>
--- a/datasets/cruise_ship.xlsx
+++ b/datasets/cruise_ship.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meredith.dodd\Documents\Data Science\105 Intermediate Statistics\Lesson 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c00f00ae0cfa65db/Documents/GitHub/CurriculumPlayground/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{574D2981-922B-4930-8ACB-9DA49C564551}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{574D2981-922B-4930-8ACB-9DA49C564551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0EF257C1-691A-43D6-AF92-3AF0D8E3A5DD}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -905,12 +903,12 @@
       <selection pane="bottomLeft" activeCell="J160" sqref="J160"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.7265625" customWidth="1"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -942,7 +940,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -974,7 +972,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1006,7 +1004,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1038,7 +1036,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1070,7 +1068,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1102,7 +1100,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1134,7 +1132,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1166,7 +1164,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1198,7 +1196,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1230,7 +1228,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1262,7 +1260,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1294,7 +1292,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1326,7 +1324,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -1358,7 +1356,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1390,7 +1388,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1422,7 +1420,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1454,7 +1452,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1486,7 +1484,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1518,7 +1516,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1550,7 +1548,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1582,7 +1580,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -1614,7 +1612,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1646,7 +1644,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1678,7 +1676,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -1710,7 +1708,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -1742,7 +1740,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1774,7 +1772,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1806,7 +1804,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1838,7 +1836,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -1870,7 +1868,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -1902,7 +1900,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -1934,7 +1932,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -1966,7 +1964,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -1998,7 +1996,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -2030,7 +2028,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -2062,7 +2060,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -2094,7 +2092,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -2126,7 +2124,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>56</v>
       </c>
@@ -2158,7 +2156,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -2190,7 +2188,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>57</v>
       </c>
@@ -2222,7 +2220,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>55</v>
       </c>
@@ -2254,7 +2252,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -2286,7 +2284,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -2318,7 +2316,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -2350,7 +2348,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -2382,7 +2380,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -2414,7 +2412,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -2446,7 +2444,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>62</v>
       </c>
@@ -2478,7 +2476,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>98</v>
       </c>
@@ -2510,7 +2508,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>63</v>
       </c>
@@ -2542,7 +2540,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>66</v>
       </c>
@@ -2574,7 +2572,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>65</v>
       </c>
@@ -2606,7 +2604,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>68</v>
       </c>
@@ -2638,7 +2636,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>81</v>
       </c>
@@ -2670,7 +2668,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>69</v>
       </c>
@@ -2702,7 +2700,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -2734,7 +2732,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>71</v>
       </c>
@@ -2766,7 +2764,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>72</v>
       </c>
@@ -2798,7 +2796,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>73</v>
       </c>
@@ -2830,7 +2828,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>74</v>
       </c>
@@ -2862,7 +2860,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>75</v>
       </c>
@@ -2894,7 +2892,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>77</v>
       </c>
@@ -2926,7 +2924,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>78</v>
       </c>
@@ -2958,7 +2956,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>79</v>
       </c>
@@ -2990,7 +2988,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>80</v>
       </c>
@@ -3022,7 +3020,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>82</v>
       </c>
@@ -3054,7 +3052,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>83</v>
       </c>
@@ -3086,7 +3084,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>90</v>
       </c>
@@ -3118,7 +3116,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>84</v>
       </c>
@@ -3150,7 +3148,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>85</v>
       </c>
@@ -3182,7 +3180,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>86</v>
       </c>
@@ -3214,7 +3212,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>87</v>
       </c>
@@ -3246,7 +3244,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>88</v>
       </c>
@@ -3278,7 +3276,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>89</v>
       </c>
@@ -3310,7 +3308,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>94</v>
       </c>
@@ -3342,7 +3340,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>95</v>
       </c>
@@ -3374,7 +3372,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>96</v>
       </c>
@@ -3406,7 +3404,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>105</v>
       </c>
@@ -3438,7 +3436,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>97</v>
       </c>
@@ -3470,7 +3468,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>100</v>
       </c>
@@ -3502,7 +3500,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>93</v>
       </c>
@@ -3534,7 +3532,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>92</v>
       </c>
@@ -3566,7 +3564,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>101</v>
       </c>
@@ -3598,7 +3596,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>14</v>
       </c>
@@ -3630,7 +3628,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>102</v>
       </c>
@@ -3662,7 +3660,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>103</v>
       </c>
@@ -3694,7 +3692,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>104</v>
       </c>
@@ -3726,7 +3724,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>106</v>
       </c>
@@ -3758,7 +3756,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>107</v>
       </c>
@@ -3790,7 +3788,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>108</v>
       </c>
@@ -3822,7 +3820,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>110</v>
       </c>
@@ -3854,7 +3852,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>112</v>
       </c>
@@ -3886,7 +3884,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>113</v>
       </c>
@@ -3918,7 +3916,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>114</v>
       </c>
@@ -3950,7 +3948,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>115</v>
       </c>
@@ -3982,7 +3980,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>116</v>
       </c>
@@ -4014,7 +4012,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>117</v>
       </c>
@@ -4046,7 +4044,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>121</v>
       </c>
@@ -4078,7 +4076,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>125</v>
       </c>
@@ -4110,7 +4108,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>94</v>
       </c>
@@ -4142,7 +4140,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>95</v>
       </c>
@@ -4174,7 +4172,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>122</v>
       </c>
@@ -4206,7 +4204,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>131</v>
       </c>
@@ -4238,7 +4236,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>123</v>
       </c>
@@ -4270,7 +4268,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>119</v>
       </c>
@@ -4302,7 +4300,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>126</v>
       </c>
@@ -4334,7 +4332,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>127</v>
       </c>
@@ -4366,7 +4364,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>128</v>
       </c>
@@ -4398,7 +4396,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>129</v>
       </c>
@@ -4430,7 +4428,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>124</v>
       </c>
@@ -4462,7 +4460,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>101</v>
       </c>
@@ -4494,7 +4492,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>102</v>
       </c>
@@ -4526,7 +4524,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>103</v>
       </c>
@@ -4558,7 +4556,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>130</v>
       </c>
@@ -4590,7 +4588,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>137</v>
       </c>
@@ -4622,7 +4620,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>133</v>
       </c>
@@ -4654,7 +4652,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>134</v>
       </c>
@@ -4686,7 +4684,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>135</v>
       </c>
@@ -4718,7 +4716,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>132</v>
       </c>
@@ -4750,7 +4748,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>140</v>
       </c>
@@ -4782,7 +4780,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>142</v>
       </c>
@@ -4814,7 +4812,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>150</v>
       </c>
@@ -4846,7 +4844,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>145</v>
       </c>
@@ -4878,7 +4876,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>141</v>
       </c>
@@ -4910,7 +4908,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>35</v>
       </c>
@@ -4942,7 +4940,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>146</v>
       </c>
@@ -4974,7 +4972,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>153</v>
       </c>
@@ -5006,7 +5004,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>97</v>
       </c>
@@ -5038,7 +5036,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>13</v>
       </c>
@@ -5070,7 +5068,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>152</v>
       </c>
@@ -5102,7 +5100,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>100</v>
       </c>
@@ -5134,7 +5132,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>133</v>
       </c>
@@ -5166,7 +5164,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>148</v>
       </c>
@@ -5198,7 +5196,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>134</v>
       </c>
@@ -5230,7 +5228,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>151</v>
       </c>
@@ -5262,7 +5260,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>143</v>
       </c>
@@ -5294,7 +5292,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>88</v>
       </c>
@@ -5326,7 +5324,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>144</v>
       </c>
@@ -5358,7 +5356,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>149</v>
       </c>
@@ -5390,7 +5388,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>139</v>
       </c>
@@ -5422,7 +5420,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>147</v>
       </c>
@@ -5454,7 +5452,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>132</v>
       </c>
@@ -5486,7 +5484,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>13</v>
       </c>
@@ -5518,7 +5516,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>5</v>
       </c>
@@ -5550,7 +5548,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>14</v>
       </c>
@@ -5582,7 +5580,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>155</v>
       </c>
@@ -5614,7 +5612,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>156</v>
       </c>
@@ -5646,7 +5644,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>157</v>
       </c>
@@ -5678,7 +5676,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>104</v>
       </c>
@@ -5710,7 +5708,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>163</v>
       </c>
@@ -5742,7 +5740,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>160</v>
       </c>
@@ -5774,7 +5772,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>161</v>
       </c>
@@ -5806,7 +5804,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>162</v>
       </c>
@@ -5838,7 +5836,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>164</v>
       </c>
@@ -5870,7 +5868,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>159</v>
       </c>
@@ -5902,7 +5900,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>14</v>
       </c>
@@ -5934,7 +5932,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>102</v>
       </c>
@@ -5966,7 +5964,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>165</v>
       </c>
@@ -6005,28 +6003,4 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>